<commit_message>
adicionado rundeck depencia no arquivo pom
</commit_message>
<xml_diff>
--- a/src/test/resources/produtos/massas/honda/planilha_veiculos_base.xlsx
+++ b/src/test/resources/produtos/massas/honda/planilha_veiculos_base.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\denis\Desktop\GitHub\automacao_honda\src\test\resources\produtos\massas\honda\"/>
     </mc:Choice>
@@ -16,7 +16,7 @@
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="17">
   <si>
     <t>entrada</t>
   </si>
@@ -64,15 +64,25 @@
   <si>
     <t>2016 Gasolina</t>
   </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>Falha</t>
+  </si>
+  <si>
+    <t>R$ 37.989,00</t>
+  </si>
+  <si>
+    <t>R$ 52.825,00</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="1">
-    <numFmt numFmtId="8" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00"/>
-  </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -121,7 +131,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="294">
     <border>
       <left/>
       <right/>
@@ -144,11 +154,1367 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -162,15 +1528,88 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="61" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="65" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="69" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="73" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="77" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="81" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="85" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="89" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="93" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="97" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="101" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="105" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="109" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="113" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="117" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="121" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="125" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="129" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="133" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="137" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="141" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="145" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="149" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="153" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="157" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="161" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="165" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="169" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="173" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="177" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="181" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="185" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="189" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="193" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="197" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="201" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="205" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="209" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="213" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="217" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="221" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="225" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="229" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="233" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="237" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="241" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="245" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="249" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="253" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="257" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="261" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="265" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="269" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="273" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="277" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="281" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="285" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="289" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="293" xfId="0" applyBorder="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -454,30 +1893,30 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="39.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="37" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="9.7109375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="39.140625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="16.140625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="37.0" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="7" t="s">
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="7"/>
+      <c r="F1" s="10"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -512,8 +1951,12 @@
       <c r="D3" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="4"/>
-      <c r="F3" s="5"/>
+      <c r="E3" s="77" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="78" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
@@ -528,8 +1971,12 @@
       <c r="D4" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="4"/>
-      <c r="F4" s="5"/>
+      <c r="E4" s="81" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="82" t="s">
+        <v>16</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
massa teste honda atualizada
</commit_message>
<xml_diff>
--- a/src/test/resources/produtos/massas/honda/planilha_veiculos_base.xlsx
+++ b/src/test/resources/produtos/massas/honda/planilha_veiculos_base.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
   <si>
     <t>entrada</t>
   </si>
@@ -69,12 +69,6 @@
   </si>
   <si>
     <t>BIZ 110i</t>
-  </si>
-  <si>
-    <t>CB 1000R/ABS</t>
-  </si>
-  <si>
-    <t>Zero KM</t>
   </si>
 </sst>
 </file>
@@ -186,17 +180,17 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -478,10 +472,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -495,16 +489,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="5" t="s">
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="5"/>
+      <c r="F1" s="7"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -527,68 +521,52 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="6"/>
-      <c r="F3" s="7"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="5"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="6"/>
-      <c r="F4" s="7"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="5"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="4">
         <v>2020</v>
       </c>
-      <c r="E5" s="6"/>
-      <c r="F5" s="7"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="E6" s="6"/>
-      <c r="F6" s="7"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
removido 1 linha planilha massa
</commit_message>
<xml_diff>
--- a/src/test/resources/produtos/massas/honda/planilha_veiculos_base.xlsx
+++ b/src/test/resources/produtos/massas/honda/planilha_veiculos_base.xlsx
@@ -1,22 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\denis\Desktop\GitHub\automacao_honda\src\test\resources\produtos\massas\honda\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
   </bookViews>
   <sheets>
     <sheet name="Carros" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="124519"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>entrada</t>
   </si>
@@ -57,25 +52,16 @@
   </si>
   <si>
     <t>2016 Gasolina</t>
-  </si>
-  <si>
-    <t>moto</t>
-  </si>
-  <si>
-    <t>Zero KM</t>
-  </si>
-  <si>
-    <t>CG 160 START</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
     <numFmt numFmtId="8" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -249,7 +235,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -284,7 +270,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -461,21 +447,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="11" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1" collapsed="1"/>
@@ -485,7 +471,7 @@
     <col min="6" max="6" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -497,7 +483,7 @@
       </c>
       <c r="F1" s="7"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -517,7 +503,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6">
       <c r="A3" s="4" t="s">
         <v>8</v>
       </c>
@@ -532,22 +518,6 @@
       </c>
       <c r="E3" s="4"/>
       <c r="F3" s="5"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4" s="4"/>
-      <c r="F4" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>